<commit_message>
Corrects bug when unicode attribute is null
</commit_message>
<xml_diff>
--- a/SegoeMDL2AssetsAlternative/font.xlsx
+++ b/SegoeMDL2AssetsAlternative/font.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual_Studio\Projects\SvgFont2Files\SvgFont2Files\SegoeMDL2AssetsAlternative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual_Studio\Projects\SvgFont2Files\SegoeMDL2AssetsAlternative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C58AFCB-6372-43B8-988B-3043956205A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484D9A84-4FAF-44BB-AEE1-7D07F78D1354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Font" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3570" uniqueCount="3052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3576" uniqueCount="3054">
   <si>
     <t>Name</t>
   </si>
@@ -9186,6 +9186,12 @@
   </si>
   <si>
     <t>&amp;#xf25a;</t>
+  </si>
+  <si>
+    <t>&amp;#xf02f;</t>
+  </si>
+  <si>
+    <t>&amp;#xf412;</t>
   </si>
 </sst>
 </file>
@@ -10029,8 +10035,8 @@
   <dimension ref="A1:D1553"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C192" sqref="C192"/>
+      <pane ySplit="1" topLeftCell="A718" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B736" sqref="B736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13549,6 +13555,12 @@
       <c r="A265" t="s">
         <v>156</v>
       </c>
+      <c r="B265" t="s">
+        <v>2728</v>
+      </c>
+      <c r="C265" t="s">
+        <v>3052</v>
+      </c>
       <c r="D265" t="s">
         <v>157</v>
       </c>
@@ -16213,6 +16225,12 @@
       <c r="A598" t="s">
         <v>822</v>
       </c>
+      <c r="B598" t="s">
+        <v>2728</v>
+      </c>
+      <c r="C598" t="s">
+        <v>3042</v>
+      </c>
       <c r="D598" t="s">
         <v>823</v>
       </c>
@@ -17316,6 +17334,12 @@
     <row r="736" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
         <v>1098</v>
+      </c>
+      <c r="B736" t="s">
+        <v>2729</v>
+      </c>
+      <c r="C736" t="s">
+        <v>3053</v>
       </c>
       <c r="D736" t="s">
         <v>1099</v>

</xml_diff>